<commit_message>
users validation, tabelas aula turmadisciplina, add button test
</commit_message>
<xml_diff>
--- a/App/Controllers/Excel/Professor.xlsx
+++ b/App/Controllers/Excel/Professor.xlsx
@@ -11,24 +11,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>JuliaDelfino</t>
-  </si>
-  <si>
-    <t>JuliaDelfino@gmail.com</t>
-  </si>
-  <si>
-    <t>Luis Esteves</t>
-  </si>
-  <si>
-    <t>LuisEsteves@gmail.com</t>
-  </si>
-  <si>
-    <t>luisa Rosado</t>
-  </si>
-  <si>
-    <t>luisaRosado@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+  <si>
+    <t>Maria Luísa Pedro Brito da Torre</t>
+  </si>
+  <si>
+    <t>123456789@gmail.com</t>
+  </si>
+  <si>
+    <t>MariaLuisa123</t>
+  </si>
+  <si>
+    <t>Júlia Maria da Rocha Vilaverde Justino</t>
+  </si>
+  <si>
+    <t>235689741@gmail.com</t>
+  </si>
+  <si>
+    <t>JuliaMaria123</t>
+  </si>
+  <si>
+    <t>Elisabete Cristina Simões Lopes</t>
+  </si>
+  <si>
+    <t>102543687@gmail.com</t>
+  </si>
+  <si>
+    <t>ElisabeteCristina123</t>
+  </si>
+  <si>
+    <t>Paula Cristina Rodrigues Miranda</t>
+  </si>
+  <si>
+    <t>159126321@gmail.com</t>
+  </si>
+  <si>
+    <t>PaulaCristina123</t>
+  </si>
+  <si>
+    <t>Luís Miguel Lopes de Oliveira Esteves</t>
+  </si>
+  <si>
+    <t>123456871@gmail.com</t>
+  </si>
+  <si>
+    <t>LuisMiguel123</t>
+  </si>
+  <si>
+    <t>António Paulo Duarte Gomes de Abreu</t>
+  </si>
+  <si>
+    <t>456781235@gmial.com</t>
+  </si>
+  <si>
+    <t>AntonioPaulo123</t>
+  </si>
+  <si>
+    <t>Manuel Mota Ferreira</t>
+  </si>
+  <si>
+    <t>581324610@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelMota123</t>
+  </si>
+  <si>
+    <t>Vítor Manuel Teles Rodrigues</t>
+  </si>
+  <si>
+    <t>468134129@gmail.com</t>
+  </si>
+  <si>
+    <t>VitorManuel123</t>
+  </si>
+  <si>
+    <t>Dulce Helena Pereira Costa</t>
+  </si>
+  <si>
+    <t>687459213@gmail.com</t>
+  </si>
+  <si>
+    <t>DulceHelena123</t>
+  </si>
+  <si>
+    <t>Jorge Manuel Martins</t>
+  </si>
+  <si>
+    <t>594751364@gmail.com</t>
+  </si>
+  <si>
+    <t>JorgeManuel123</t>
+  </si>
+  <si>
+    <t>José Garcia Costa Correia de Sousa</t>
+  </si>
+  <si>
+    <t>254163987@gmail.com</t>
+  </si>
+  <si>
+    <t>JoseGarcia123</t>
+  </si>
+  <si>
+    <t>Fernando Manuel Valente</t>
+  </si>
+  <si>
+    <t>654751239@gmail.com</t>
+  </si>
+  <si>
+    <t>FernandoManuel123</t>
+  </si>
+  <si>
+    <t>Dina Maria Morgado Salvador</t>
+  </si>
+  <si>
+    <t>541687913@gmail.com</t>
+  </si>
+  <si>
+    <t>DinaMaria123</t>
+  </si>
+  <si>
+    <t>André Miguel Namorado Canhoto Antunes</t>
+  </si>
+  <si>
+    <t>621873498@gmail.com</t>
+  </si>
+  <si>
+    <t>AndreMiguel123</t>
   </si>
 </sst>
 </file>
@@ -41,7 +149,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -51,18 +162,27 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <right/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -287,43 +407,194 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>1.23456789E8</v>
       </c>
-      <c r="D1" s="1">
-        <v>123.0</v>
-      </c>
-      <c r="E1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
         <v>2.35689741E8</v>
       </c>
-      <c r="D2" s="1">
-        <v>456.0</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
         <v>1.02543687E8</v>
       </c>
-      <c r="D3" s="1">
-        <v>789.0</v>
-      </c>
-      <c r="E3" s="1"/>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.59126321E8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.23456871E8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.56781235E8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.8132461E8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.68134129E8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6.87459213E8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.94751364E8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.54163987E8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6.54751239E8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.41687913E8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.21873498E8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>